<commit_message>
Acabamos el tema de Mybatis con Manolo Empezamos con Hibernate 17/04/2018 11:45
</commit_message>
<xml_diff>
--- a/Documentos.xlsx
+++ b/Documentos.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="17">
   <si>
     <t>doc1</t>
   </si>
@@ -53,6 +53,27 @@
   </si>
   <si>
     <t>Tue Apr 10 12:45:23 CEST 2018</t>
+  </si>
+  <si>
+    <t>nombre</t>
+  </si>
+  <si>
+    <t>Tue Apr 17 09:52:40 CEST 2018</t>
+  </si>
+  <si>
+    <t>Tue Apr 17 09:52:55 CEST 2018</t>
+  </si>
+  <si>
+    <t>Tue Apr 17 09:53:27 CEST 2018</t>
+  </si>
+  <si>
+    <t>Tue Apr 17 09:59:00 CEST 2018</t>
+  </si>
+  <si>
+    <t>Tue Apr 17 10:01:15 CEST 2018</t>
+  </si>
+  <si>
+    <t>Tue Apr 17 10:01:22 CEST 2018</t>
   </si>
 </sst>
 </file>
@@ -175,7 +196,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:F11"/>
+  <dimension ref="A2:F17"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A11" activeCellId="0" pane="topLeft" sqref="A11"/>
@@ -353,6 +374,108 @@
         <v>9</v>
       </c>
       <c r="E11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="B12" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="B13" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="B14" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="B15" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="B16" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="B17" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" t="s">
         <v>2</v>
       </c>
     </row>
@@ -372,7 +495,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:F5"/>
+  <dimension ref="A2:F11"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A5" activeCellId="0" pane="topLeft" sqref="A5"/>
@@ -450,6 +573,108 @@
         <v>9</v>
       </c>
       <c r="E5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>